<commit_message>
excel update első 3 use-case
</commit_message>
<xml_diff>
--- a/USE_CASE_LEVEZETES.xlsx
+++ b/USE_CASE_LEVEZETES.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\csern\OneDrive\Dokumentumok\GitHub\SzoftTech\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\goczi\Desktop\5. félév\Szoftvertechnológia\repo\SzoftTech\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F689FD8-1158-4700-BB59-2B3B084E0629}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1"/>
+    <workbookView xWindow="-2760" yWindow="-14640" windowWidth="21600" windowHeight="11295" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Use-case" sheetId="1" r:id="rId1"/>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="329" uniqueCount="171">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="333" uniqueCount="165">
   <si>
     <t>Use case name</t>
   </si>
@@ -292,81 +293,24 @@
     <t>4.</t>
   </si>
   <si>
-    <t>3.1</t>
-  </si>
-  <si>
-    <t>3.2</t>
-  </si>
-  <si>
-    <t>A rendszer jelzi, hogy melyik mező nem lett kitöltve.</t>
-  </si>
-  <si>
     <t>4.1</t>
   </si>
   <si>
     <t>4.2</t>
   </si>
   <si>
-    <t>A rendszer hibaüzenetet dob.</t>
-  </si>
-  <si>
-    <t>Új beteg létrehozása</t>
-  </si>
-  <si>
-    <t>Az orvos létre tudja hozni a beteg fiókját.</t>
-  </si>
-  <si>
     <t>Az orvos legyen bejelentkezve</t>
   </si>
   <si>
     <t>Orvos</t>
   </si>
   <si>
-    <t>Az orvos létre akar hozni egy új beteg-fiókot.</t>
-  </si>
-  <si>
-    <t>Az orvos utasítást ad a rendszernek, hogy új beteg-fiókot akar létrehozni.</t>
-  </si>
-  <si>
-    <t>A rendszer visszaad egy kitöltendő felületet.</t>
-  </si>
-  <si>
-    <t>Az orvos visszaküldi a kitöltött regisztrációs felületet.</t>
-  </si>
-  <si>
-    <t>A rendszer ellenőrzi a külső adatbázisban, hogy van-e ilyen felhasználó, ha nincs akkor regisztrál egy új beteg felhasználót.</t>
-  </si>
-  <si>
-    <t>Hiányosan küldi vissza az orvos az űrlapot.</t>
-  </si>
-  <si>
-    <t>Már létezik ilyen beteg.</t>
-  </si>
-  <si>
     <t>Az orvos receptet szeretne felírni a betegnek.</t>
   </si>
   <si>
     <t>Az orvos utasítást ad a rendszernek, hogy receptet akar felírni.</t>
   </si>
   <si>
-    <t>Az orvos visszaküldi a kitöltött recept sablont.</t>
-  </si>
-  <si>
-    <t>A rendszer visszaad egy kitöltendő sablont.</t>
-  </si>
-  <si>
-    <t>A rendszer hozzáadja a beteg recept listájához.</t>
-  </si>
-  <si>
-    <t>Hiányosan küldi vissza az orvos a receptet.</t>
-  </si>
-  <si>
-    <t>Nem adja hozzá a receptet a listához.</t>
-  </si>
-  <si>
-    <t>Új recept hozzáadása</t>
-  </si>
-  <si>
     <t>Recept megtekintése</t>
   </si>
   <si>
@@ -436,18 +380,6 @@
     <t>A rendszer hibát dob, mivel nem volt kiválasztva recept</t>
   </si>
   <si>
-    <t>4.1/a</t>
-  </si>
-  <si>
-    <t>4.2/a</t>
-  </si>
-  <si>
-    <t>4.2/b</t>
-  </si>
-  <si>
-    <t>Nem elérhető az adatbázis</t>
-  </si>
-  <si>
     <t>2.1</t>
   </si>
   <si>
@@ -472,9 +404,6 @@
     <t>5.3</t>
   </si>
   <si>
-    <t>Sikeres sikertelen lefutás.</t>
-  </si>
-  <si>
     <t>Recept megtekintése orvosi felhasználóval</t>
   </si>
   <si>
@@ -484,21 +413,12 @@
     <t>Sikeres lefutás</t>
   </si>
   <si>
-    <t>Az orvos létrehoz egy beteg felhasználót.</t>
-  </si>
-  <si>
     <t>Sikertelen lefutás</t>
   </si>
   <si>
-    <t>Az applikáció visszautasítja a regisztrációt.</t>
-  </si>
-  <si>
     <t>Az orvos hozzáad egy új receptet a beteghez.</t>
   </si>
   <si>
-    <t>Az applikáció visszautasítja a recept hozzáadását.</t>
-  </si>
-  <si>
     <t>Orvos/gyógyszertár legyen bejelentkezve</t>
   </si>
   <si>
@@ -538,18 +458,6 @@
     <t>Beteg törlése</t>
   </si>
   <si>
-    <t>Az orvos törölni tudja hozni a beteg fiókját.</t>
-  </si>
-  <si>
-    <t>Az orvos sikeresen törölte a felhasználói fiókot</t>
-  </si>
-  <si>
-    <t>A fiók bennt maradt a rendszerben</t>
-  </si>
-  <si>
-    <t>Az orvos törölni akar egy felhasználói fiókot</t>
-  </si>
-  <si>
     <t>A beteg részéről egy igény benyújtása</t>
   </si>
   <si>
@@ -566,12 +474,87 @@
   </si>
   <si>
     <t>A beteg igényt szeretne benyújtani gyógyszerekre</t>
+  </si>
+  <si>
+    <t>Beteg felvétele</t>
+  </si>
+  <si>
+    <t>Orvos fel tudja venni a beteget</t>
+  </si>
+  <si>
+    <t>Az orvos listájára sikeresen felkerül a beteg</t>
+  </si>
+  <si>
+    <t>Az orvos beteg listája változatlan marad</t>
+  </si>
+  <si>
+    <t>Orvos fel akarja venni a beteget</t>
+  </si>
+  <si>
+    <t>Az orvos utasítást ad a rendszernek, beteg felvételére</t>
+  </si>
+  <si>
+    <t>A rendszer visszaad egy listát a betegekkel</t>
+  </si>
+  <si>
+    <t>Rendszer rögzíti az orvos beteg listájára a vélasztott beteget.</t>
+  </si>
+  <si>
+    <t>Az orvos kiválasztja a beteget</t>
+  </si>
+  <si>
+    <t>A beteg már fel van véve az adott orvoshoz</t>
+  </si>
+  <si>
+    <t>Az orvos törölni tudja az álltala felvett betegeket a listájáról</t>
+  </si>
+  <si>
+    <t>Az orvos listájáról törlődik a beteg</t>
+  </si>
+  <si>
+    <t>Az orvos törölni akar egy beteget a listájáról</t>
+  </si>
+  <si>
+    <t>Az orvos utasítást ad a rendszernek beteg törlésére</t>
+  </si>
+  <si>
+    <t>A rendszer kilistázza az orvoshoz tartozó betegeket</t>
+  </si>
+  <si>
+    <t>Az orvos kiválasztja a törölni kívánt beteget</t>
+  </si>
+  <si>
+    <t>A rendszer törli a beteget az adott orvos listájáról</t>
+  </si>
+  <si>
+    <t>Nincs még az orvosnak beteg a listáján</t>
+  </si>
+  <si>
+    <t>Új recept létrehozása</t>
+  </si>
+  <si>
+    <t>A rendszer kilistázza az orvos betegeit</t>
+  </si>
+  <si>
+    <t>Orvos kiválasztja a felírni kívánt gyógyszert.</t>
+  </si>
+  <si>
+    <t>Beteg recept listájára felkerül az új recept.</t>
+  </si>
+  <si>
+    <t>A rendszer kilistázza az elérhető gyógyszereket</t>
+  </si>
+  <si>
+    <t>Hiba feljegyzése</t>
+  </si>
+  <si>
+    <t>A beteg recept listája változatlan marad</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -900,7 +883,7 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1181,21 +1164,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B56"/>
   <sheetViews>
     <sheetView topLeftCell="A31" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="35.6640625" customWidth="1"/>
+    <col min="1" max="1" width="35.7109375" customWidth="1"/>
     <col min="2" max="2" width="71" customWidth="1"/>
-    <col min="5" max="5" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -1203,7 +1186,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
         <v>2</v>
       </c>
@@ -1211,7 +1194,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="37" t="s">
         <v>4</v>
       </c>
@@ -1219,11 +1202,11 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="37"/>
       <c r="B4" s="38"/>
     </row>
-    <row r="5" spans="1:2" ht="37.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" ht="37.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
         <v>6</v>
       </c>
@@ -1231,7 +1214,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
         <v>8</v>
       </c>
@@ -1239,7 +1222,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
         <v>10</v>
       </c>
@@ -1247,7 +1230,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
         <v>27</v>
       </c>
@@ -1255,7 +1238,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
         <v>13</v>
       </c>
@@ -1263,7 +1246,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
         <v>17</v>
       </c>
@@ -1271,7 +1254,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="9" t="s">
         <v>16</v>
       </c>
@@ -1279,7 +1262,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:2" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="10" t="s">
         <v>19</v>
       </c>
@@ -1287,10 +1270,10 @@
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B13" s="1"/>
     </row>
-    <row r="14" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="6" t="s">
         <v>0</v>
       </c>
@@ -1298,7 +1281,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="8" t="s">
         <v>2</v>
       </c>
@@ -1306,7 +1289,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="37" t="s">
         <v>4</v>
       </c>
@@ -1314,11 +1297,11 @@
         <v>23</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="37"/>
       <c r="B17" s="38"/>
     </row>
-    <row r="18" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="9" t="s">
         <v>6</v>
       </c>
@@ -1326,7 +1309,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="19" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="9" t="s">
         <v>24</v>
       </c>
@@ -1334,7 +1317,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="20" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A20" s="11" t="s">
         <v>28</v>
       </c>
@@ -1342,7 +1325,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="21" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="11" t="s">
         <v>29</v>
       </c>
@@ -1350,7 +1333,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="22" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A22" s="11" t="s">
         <v>31</v>
       </c>
@@ -1358,7 +1341,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="23" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="11" t="s">
         <v>33</v>
       </c>
@@ -1366,7 +1349,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="24" spans="1:2" ht="87" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:2" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="12" t="s">
         <v>19</v>
       </c>
@@ -1374,11 +1357,11 @@
         <v>35</v>
       </c>
     </row>
-    <row r="25" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="1"/>
       <c r="B25" s="1"/>
     </row>
-    <row r="26" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="6" t="s">
         <v>0</v>
       </c>
@@ -1386,7 +1369,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="8" t="s">
         <v>2</v>
       </c>
@@ -1394,7 +1377,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="37" t="s">
         <v>4</v>
       </c>
@@ -1402,11 +1385,11 @@
         <v>39</v>
       </c>
     </row>
-    <row r="29" spans="1:2" ht="0.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:2" ht="0.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="37"/>
       <c r="B29" s="38"/>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" s="9" t="s">
         <v>6</v>
       </c>
@@ -1414,7 +1397,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="31" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" s="9" t="s">
         <v>24</v>
       </c>
@@ -1422,7 +1405,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="32" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A32" s="11" t="s">
         <v>41</v>
       </c>
@@ -1430,7 +1413,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="11" t="s">
         <v>43</v>
       </c>
@@ -1438,7 +1421,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="34" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A34" s="11" t="s">
         <v>19</v>
       </c>
@@ -1446,7 +1429,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="35" spans="1:2" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:2" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="12" t="s">
         <v>46</v>
       </c>
@@ -1454,11 +1437,11 @@
         <v>47</v>
       </c>
     </row>
-    <row r="36" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="2"/>
       <c r="B36" s="1"/>
     </row>
-    <row r="37" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="6" t="s">
         <v>0</v>
       </c>
@@ -1466,7 +1449,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" s="8" t="s">
         <v>2</v>
       </c>
@@ -1474,7 +1457,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" s="37" t="s">
         <v>4</v>
       </c>
@@ -1482,11 +1465,11 @@
         <v>50</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" s="37"/>
       <c r="B40" s="38"/>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" s="9" t="s">
         <v>6</v>
       </c>
@@ -1494,7 +1477,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="42" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A42" s="9" t="s">
         <v>24</v>
       </c>
@@ -1502,7 +1485,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="43" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A43" s="11" t="s">
         <v>52</v>
       </c>
@@ -1510,7 +1493,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" s="11" t="s">
         <v>54</v>
       </c>
@@ -1518,7 +1501,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="45" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A45" s="11" t="s">
         <v>57</v>
       </c>
@@ -1526,7 +1509,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="46" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A46" s="11" t="s">
         <v>19</v>
       </c>
@@ -1534,7 +1517,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A47" s="11" t="s">
         <v>60</v>
       </c>
@@ -1542,7 +1525,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" s="11" t="s">
         <v>61</v>
       </c>
@@ -1550,7 +1533,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" s="13" t="s">
         <v>63</v>
       </c>
@@ -1558,18 +1541,18 @@
         <v>64</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" s="17"/>
       <c r="B50" s="18"/>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B51" s="1"/>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" s="16"/>
       <c r="B52" s="1"/>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B56" s="15"/>
     </row>
   </sheetData>
@@ -1589,41 +1572,41 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G113"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:G109"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
-      <selection activeCell="B89" sqref="B89"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.33203125" style="20" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="54.109375" style="21" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.109375" style="19"/>
-    <col min="4" max="4" width="19.6640625" style="19" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="53.33203125" style="19" customWidth="1"/>
-    <col min="6" max="6" width="9.109375" style="19"/>
-    <col min="7" max="7" width="37.88671875" style="19" customWidth="1"/>
+    <col min="1" max="1" width="17.28515625" style="20" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="54.140625" style="21" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.140625" style="19"/>
+    <col min="4" max="4" width="19.7109375" style="19" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="53.28515625" style="19" customWidth="1"/>
+    <col min="6" max="6" width="9.140625" style="19"/>
+    <col min="7" max="7" width="37.85546875" style="19" customWidth="1"/>
     <col min="8" max="8" width="52" style="19" customWidth="1"/>
-    <col min="9" max="16384" width="9.109375" style="19"/>
+    <col min="9" max="16384" width="9.140625" style="19"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="31" t="s">
         <v>65</v>
       </c>
       <c r="B1" s="26" t="s">
-        <v>85</v>
+        <v>140</v>
       </c>
       <c r="D1" s="31" t="s">
         <v>65</v>
       </c>
       <c r="E1" s="26" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="32" t="s">
         <v>66</v>
       </c>
@@ -1633,108 +1616,105 @@
       </c>
       <c r="E2" s="27"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="33" t="s">
         <v>67</v>
       </c>
       <c r="B3" s="28" t="s">
-        <v>86</v>
+        <v>141</v>
       </c>
       <c r="D3" s="33" t="s">
         <v>67</v>
       </c>
       <c r="E3" s="28" t="s">
-        <v>161</v>
-      </c>
-      <c r="G3" s="19" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="33" t="s">
         <v>68</v>
       </c>
       <c r="B4" s="28" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="D4" s="33" t="s">
         <v>68</v>
       </c>
       <c r="E4" s="28" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="33" t="s">
+        <v>118</v>
+      </c>
+      <c r="B5" s="28" t="s">
         <v>142</v>
       </c>
-      <c r="B5" s="28" t="s">
+      <c r="D5" s="33" t="s">
+        <v>118</v>
+      </c>
+      <c r="E5" s="28" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="33" t="s">
+        <v>119</v>
+      </c>
+      <c r="B6" s="28" t="s">
         <v>143</v>
       </c>
-      <c r="D5" s="33" t="s">
-        <v>142</v>
-      </c>
-      <c r="E5" s="28" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A6" s="33" t="s">
-        <v>144</v>
-      </c>
-      <c r="B6" s="28" t="s">
-        <v>145</v>
-      </c>
       <c r="D6" s="33" t="s">
-        <v>144</v>
+        <v>119</v>
       </c>
       <c r="E6" s="28" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="34" t="s">
         <v>69</v>
       </c>
       <c r="B7" s="28" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="D7" s="34" t="s">
         <v>69</v>
       </c>
       <c r="E7" s="28" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="34" t="s">
         <v>70</v>
       </c>
       <c r="B8" s="28" t="s">
-        <v>75</v>
+        <v>89</v>
       </c>
       <c r="D8" s="34" t="s">
         <v>70</v>
       </c>
       <c r="E8" s="28" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="34" t="s">
         <v>71</v>
       </c>
       <c r="B9" s="28" t="s">
-        <v>89</v>
+        <v>144</v>
       </c>
       <c r="D9" s="34" t="s">
         <v>71</v>
       </c>
       <c r="E9" s="28" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="34" t="s">
         <v>72</v>
       </c>
@@ -1744,962 +1724,945 @@
       </c>
       <c r="E10" s="28"/>
     </row>
-    <row r="11" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="35" t="s">
         <v>74</v>
       </c>
       <c r="B11" s="28" t="s">
-        <v>90</v>
-      </c>
-      <c r="D11" s="35"/>
-      <c r="E11" s="28"/>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+        <v>145</v>
+      </c>
+      <c r="D11" s="35" t="s">
+        <v>74</v>
+      </c>
+      <c r="E11" s="28" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="35" t="s">
         <v>76</v>
       </c>
       <c r="B12" s="28" t="s">
-        <v>91</v>
-      </c>
-      <c r="D12" s="35"/>
-      <c r="E12" s="28"/>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+        <v>146</v>
+      </c>
+      <c r="D12" s="35" t="s">
+        <v>76</v>
+      </c>
+      <c r="E12" s="28" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="35" t="s">
         <v>77</v>
       </c>
       <c r="B13" s="28" t="s">
-        <v>92</v>
-      </c>
-      <c r="D13" s="35"/>
-      <c r="E13" s="28"/>
-    </row>
-    <row r="14" spans="1:7" ht="46.8" x14ac:dyDescent="0.3">
+        <v>148</v>
+      </c>
+      <c r="D13" s="35" t="s">
+        <v>77</v>
+      </c>
+      <c r="E13" s="28" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="35" t="s">
         <v>78</v>
       </c>
       <c r="B14" s="28" t="s">
-        <v>93</v>
-      </c>
-      <c r="D14" s="35"/>
-      <c r="E14" s="28"/>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+        <v>147</v>
+      </c>
+      <c r="D14" s="35" t="s">
+        <v>78</v>
+      </c>
+      <c r="E14" s="28" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="34" t="s">
         <v>73</v>
       </c>
       <c r="B15" s="28"/>
-      <c r="D15" s="34"/>
+      <c r="D15" s="34" t="s">
+        <v>73</v>
+      </c>
       <c r="E15" s="28"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="35" t="s">
         <v>79</v>
       </c>
       <c r="B16" s="28" t="s">
+        <v>149</v>
+      </c>
+      <c r="D16" s="35" t="s">
+        <v>108</v>
+      </c>
+      <c r="E16" s="28" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="36" t="s">
+        <v>80</v>
+      </c>
+      <c r="B17" s="29" t="s">
+        <v>163</v>
+      </c>
+      <c r="D17" s="36" t="s">
+        <v>109</v>
+      </c>
+      <c r="E17" s="29" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="19"/>
+      <c r="B18" s="19"/>
+    </row>
+    <row r="19" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="31" t="s">
+        <v>65</v>
+      </c>
+      <c r="B19" s="26" t="s">
+        <v>158</v>
+      </c>
+      <c r="G19" s="39"/>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="32" t="s">
+        <v>66</v>
+      </c>
+      <c r="B20" s="27"/>
+      <c r="G20" s="39"/>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="33" t="s">
+        <v>67</v>
+      </c>
+      <c r="B21" s="28" t="s">
+        <v>86</v>
+      </c>
+      <c r="G21" s="39"/>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" s="33" t="s">
+        <v>68</v>
+      </c>
+      <c r="B22" s="28" t="s">
+        <v>81</v>
+      </c>
+      <c r="G22" s="39"/>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" s="33" t="s">
+        <v>118</v>
+      </c>
+      <c r="B23" s="28" t="s">
+        <v>120</v>
+      </c>
+      <c r="G23" s="39"/>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" s="33" t="s">
+        <v>119</v>
+      </c>
+      <c r="B24" s="28" t="s">
+        <v>164</v>
+      </c>
+      <c r="G24" s="39"/>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" s="34" t="s">
+        <v>69</v>
+      </c>
+      <c r="B25" s="28" t="s">
+        <v>82</v>
+      </c>
+      <c r="G25" s="39"/>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" s="34" t="s">
+        <v>70</v>
+      </c>
+      <c r="B26" s="28" t="s">
+        <v>89</v>
+      </c>
+      <c r="G26" s="39"/>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" s="34" t="s">
+        <v>71</v>
+      </c>
+      <c r="B27" s="28" t="s">
+        <v>83</v>
+      </c>
+      <c r="G27" s="39"/>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" s="34" t="s">
+        <v>72</v>
+      </c>
+      <c r="B28" s="28"/>
+      <c r="G28" s="39"/>
+    </row>
+    <row r="29" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A29" s="35" t="s">
+        <v>74</v>
+      </c>
+      <c r="B29" s="28" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" s="35" t="s">
+        <v>76</v>
+      </c>
+      <c r="B30" s="28" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" s="35" t="s">
+        <v>77</v>
+      </c>
+      <c r="B31" s="28" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" s="35" t="s">
+        <v>78</v>
+      </c>
+      <c r="B32" s="28" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" s="35" t="s">
+        <v>102</v>
+      </c>
+      <c r="B33" s="28" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" s="35" t="s">
+        <v>104</v>
+      </c>
+      <c r="B34" s="28" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35" s="34" t="s">
+        <v>73</v>
+      </c>
+      <c r="B35" s="28"/>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36" s="35" t="s">
+        <v>108</v>
+      </c>
+      <c r="B36" s="28" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="36" t="s">
+        <v>109</v>
+      </c>
+      <c r="B37" s="29" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="39" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="31" t="s">
+        <v>65</v>
+      </c>
+      <c r="B39" s="26" t="s">
+        <v>116</v>
+      </c>
+      <c r="D39" s="26" t="s">
+        <v>65</v>
+      </c>
+      <c r="E39" s="26" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A40" s="32" t="s">
+        <v>66</v>
+      </c>
+      <c r="B40" s="27"/>
+      <c r="D40" s="23" t="s">
+        <v>66</v>
+      </c>
+      <c r="E40" s="27"/>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A41" s="33" t="s">
+        <v>67</v>
+      </c>
+      <c r="B41" s="28" t="s">
+        <v>85</v>
+      </c>
+      <c r="D41" s="30" t="s">
+        <v>67</v>
+      </c>
+      <c r="E41" s="28" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A42" s="33" t="s">
+        <v>68</v>
+      </c>
+      <c r="B42" s="28" t="s">
+        <v>121</v>
+      </c>
+      <c r="D42" s="30" t="s">
+        <v>68</v>
+      </c>
+      <c r="E42" s="28" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A43" s="33" t="s">
+        <v>118</v>
+      </c>
+      <c r="B43" s="28" t="s">
+        <v>123</v>
+      </c>
+      <c r="D43" s="33" t="s">
+        <v>118</v>
+      </c>
+      <c r="E43" s="28" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A44" s="33" t="s">
+        <v>119</v>
+      </c>
+      <c r="B44" s="28" t="s">
+        <v>124</v>
+      </c>
+      <c r="D44" s="33" t="s">
+        <v>119</v>
+      </c>
+      <c r="E44" s="28" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A45" s="34" t="s">
+        <v>69</v>
+      </c>
+      <c r="B45" s="28" t="s">
+        <v>122</v>
+      </c>
+      <c r="D45" s="22" t="s">
+        <v>69</v>
+      </c>
+      <c r="E45" s="28" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A46" s="34" t="s">
+        <v>70</v>
+      </c>
+      <c r="B46" s="28" t="s">
+        <v>75</v>
+      </c>
+      <c r="D46" s="22" t="s">
+        <v>70</v>
+      </c>
+      <c r="E46" s="28" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A47" s="34" t="s">
+        <v>71</v>
+      </c>
+      <c r="B47" s="28" t="s">
+        <v>90</v>
+      </c>
+      <c r="D47" s="22" t="s">
+        <v>71</v>
+      </c>
+      <c r="E47" s="28" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A48" s="34" t="s">
+        <v>72</v>
+      </c>
+      <c r="B48" s="28"/>
+      <c r="D48" s="22" t="s">
+        <v>72</v>
+      </c>
+      <c r="E48" s="28"/>
+    </row>
+    <row r="49" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A49" s="35" t="s">
+        <v>74</v>
+      </c>
+      <c r="B49" s="28" t="s">
+        <v>92</v>
+      </c>
+      <c r="D49" s="24" t="s">
+        <v>74</v>
+      </c>
+      <c r="E49" s="28" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A50" s="35" t="s">
+        <v>76</v>
+      </c>
+      <c r="B50" s="28" t="s">
+        <v>93</v>
+      </c>
+      <c r="D50" s="24" t="s">
+        <v>76</v>
+      </c>
+      <c r="E50" s="28" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A51" s="35" t="s">
+        <v>77</v>
+      </c>
+      <c r="B51" s="28" t="s">
         <v>94</v>
       </c>
-      <c r="D16" s="35"/>
-      <c r="E16" s="28"/>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A17" s="35" t="s">
-        <v>80</v>
-      </c>
-      <c r="B17" s="28" t="s">
-        <v>81</v>
-      </c>
-      <c r="D17" s="35"/>
-      <c r="E17" s="28"/>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A18" s="35" t="s">
-        <v>127</v>
-      </c>
-      <c r="B18" s="28" t="s">
+      <c r="D51" s="24"/>
+      <c r="E51" s="28"/>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A52" s="35" t="s">
+        <v>78</v>
+      </c>
+      <c r="B52" s="28" t="s">
         <v>95</v>
       </c>
-      <c r="D18" s="35"/>
-      <c r="E18" s="28"/>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A19" s="35" t="s">
-        <v>128</v>
-      </c>
-      <c r="B19" s="28" t="s">
-        <v>84</v>
-      </c>
-      <c r="D19" s="35"/>
-      <c r="E19" s="28"/>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A20" s="35" t="s">
-        <v>129</v>
-      </c>
-      <c r="B20" s="28" t="s">
-        <v>130</v>
-      </c>
-      <c r="D20" s="35"/>
-      <c r="E20" s="28"/>
-    </row>
-    <row r="21" spans="1:7" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="36" t="s">
-        <v>129</v>
-      </c>
-      <c r="B21" s="29" t="s">
-        <v>84</v>
-      </c>
-      <c r="D21" s="36"/>
-      <c r="E21" s="29"/>
-    </row>
-    <row r="22" spans="1:7" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="19"/>
-      <c r="B22" s="19"/>
-    </row>
-    <row r="23" spans="1:7" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="31" t="s">
-        <v>65</v>
-      </c>
-      <c r="B23" s="26" t="s">
-        <v>103</v>
-      </c>
-      <c r="G23" s="39"/>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A24" s="32" t="s">
-        <v>66</v>
-      </c>
-      <c r="B24" s="27"/>
-      <c r="G24" s="39"/>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A25" s="33" t="s">
-        <v>67</v>
-      </c>
-      <c r="B25" s="28" t="s">
-        <v>105</v>
-      </c>
-      <c r="G25" s="39"/>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A26" s="33" t="s">
-        <v>68</v>
-      </c>
-      <c r="B26" s="28" t="s">
-        <v>87</v>
-      </c>
-      <c r="G26" s="39"/>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A27" s="33" t="s">
-        <v>142</v>
-      </c>
-      <c r="B27" s="28" t="s">
-        <v>146</v>
-      </c>
-      <c r="G27" s="39"/>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A28" s="33" t="s">
-        <v>144</v>
-      </c>
-      <c r="B28" s="28" t="s">
-        <v>147</v>
-      </c>
-      <c r="G28" s="39"/>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A29" s="34" t="s">
-        <v>69</v>
-      </c>
-      <c r="B29" s="28" t="s">
-        <v>88</v>
-      </c>
-      <c r="G29" s="39"/>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A30" s="34" t="s">
-        <v>70</v>
-      </c>
-      <c r="B30" s="28" t="s">
-        <v>75</v>
-      </c>
-      <c r="G30" s="39"/>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A31" s="34" t="s">
-        <v>71</v>
-      </c>
-      <c r="B31" s="28" t="s">
+      <c r="D52" s="24"/>
+      <c r="E52" s="28"/>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A53" s="34" t="s">
+        <v>73</v>
+      </c>
+      <c r="B53" s="28"/>
+      <c r="D53" s="22" t="s">
+        <v>73</v>
+      </c>
+      <c r="E53" s="28"/>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A54" s="35" t="s">
+        <v>108</v>
+      </c>
+      <c r="B54" s="28" t="s">
         <v>96</v>
       </c>
-      <c r="G31" s="39"/>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A32" s="34" t="s">
-        <v>72</v>
-      </c>
-      <c r="B32" s="28"/>
-      <c r="G32" s="39"/>
-    </row>
-    <row r="33" spans="1:5" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A33" s="35" t="s">
-        <v>74</v>
-      </c>
-      <c r="B33" s="28" t="s">
+      <c r="D54" s="35" t="s">
+        <v>108</v>
+      </c>
+      <c r="E54" s="28" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A55" s="35" t="s">
+        <v>109</v>
+      </c>
+      <c r="B55" s="28" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A34" s="35" t="s">
-        <v>76</v>
-      </c>
-      <c r="B34" s="28" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A35" s="35" t="s">
-        <v>77</v>
-      </c>
-      <c r="B35" s="28" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A36" s="35" t="s">
-        <v>78</v>
-      </c>
-      <c r="B36" s="28" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A37" s="34" t="s">
-        <v>73</v>
-      </c>
-      <c r="B37" s="28"/>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A38" s="35" t="s">
-        <v>79</v>
-      </c>
-      <c r="B38" s="28" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A39" s="35" t="s">
-        <v>80</v>
-      </c>
-      <c r="B39" s="28" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A40" s="35" t="s">
-        <v>82</v>
-      </c>
-      <c r="B40" s="28" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A41" s="36" t="s">
-        <v>83</v>
-      </c>
-      <c r="B41" s="29" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="43" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A43" s="31" t="s">
-        <v>65</v>
-      </c>
-      <c r="B43" s="26" t="s">
-        <v>140</v>
-      </c>
-      <c r="D43" s="26" t="s">
-        <v>65</v>
-      </c>
-      <c r="E43" s="26" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A44" s="32" t="s">
-        <v>66</v>
-      </c>
-      <c r="B44" s="27"/>
-      <c r="D44" s="23" t="s">
-        <v>66</v>
-      </c>
-      <c r="E44" s="27"/>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A45" s="33" t="s">
-        <v>67</v>
-      </c>
-      <c r="B45" s="28" t="s">
-        <v>104</v>
-      </c>
-      <c r="D45" s="30" t="s">
-        <v>67</v>
-      </c>
-      <c r="E45" s="28" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A46" s="33" t="s">
-        <v>68</v>
-      </c>
-      <c r="B46" s="28" t="s">
-        <v>148</v>
-      </c>
-      <c r="D46" s="30" t="s">
-        <v>68</v>
-      </c>
-      <c r="E46" s="28" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A47" s="33" t="s">
-        <v>142</v>
-      </c>
-      <c r="B47" s="28" t="s">
-        <v>150</v>
-      </c>
-      <c r="D47" s="33" t="s">
-        <v>142</v>
-      </c>
-      <c r="E47" s="28" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A48" s="33" t="s">
-        <v>144</v>
-      </c>
-      <c r="B48" s="28" t="s">
-        <v>151</v>
-      </c>
-      <c r="D48" s="33" t="s">
-        <v>144</v>
-      </c>
-      <c r="E48" s="28" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A49" s="34" t="s">
-        <v>69</v>
-      </c>
-      <c r="B49" s="28" t="s">
-        <v>149</v>
-      </c>
-      <c r="D49" s="22" t="s">
-        <v>69</v>
-      </c>
-      <c r="E49" s="28" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A50" s="34" t="s">
-        <v>70</v>
-      </c>
-      <c r="B50" s="28" t="s">
-        <v>75</v>
-      </c>
-      <c r="D50" s="22" t="s">
-        <v>70</v>
-      </c>
-      <c r="E50" s="28" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A51" s="34" t="s">
-        <v>71</v>
-      </c>
-      <c r="B51" s="28" t="s">
+      <c r="D55" s="35" t="s">
         <v>109</v>
       </c>
-      <c r="D51" s="22" t="s">
-        <v>71</v>
-      </c>
-      <c r="E51" s="28" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A52" s="34" t="s">
-        <v>72</v>
-      </c>
-      <c r="B52" s="28"/>
-      <c r="D52" s="22" t="s">
-        <v>72</v>
-      </c>
-      <c r="E52" s="28"/>
-    </row>
-    <row r="53" spans="1:5" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A53" s="35" t="s">
-        <v>74</v>
-      </c>
-      <c r="B53" s="28" t="s">
+      <c r="E55" s="28" t="s">
         <v>111</v>
       </c>
-      <c r="D53" s="24" t="s">
-        <v>74</v>
-      </c>
-      <c r="E53" s="28" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A54" s="35" t="s">
-        <v>76</v>
-      </c>
-      <c r="B54" s="28" t="s">
-        <v>112</v>
-      </c>
-      <c r="D54" s="24" t="s">
-        <v>76</v>
-      </c>
-      <c r="E54" s="28" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A55" s="35" t="s">
-        <v>77</v>
-      </c>
-      <c r="B55" s="28" t="s">
-        <v>113</v>
-      </c>
-      <c r="D55" s="24"/>
-      <c r="E55" s="28"/>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A56" s="35" t="s">
-        <v>78</v>
-      </c>
-      <c r="B56" s="28" t="s">
-        <v>114</v>
-      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A56" s="35"/>
+      <c r="B56" s="28"/>
       <c r="D56" s="24"/>
       <c r="E56" s="28"/>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A57" s="34" t="s">
-        <v>73</v>
-      </c>
+    <row r="57" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A57" s="35"/>
       <c r="B57" s="28"/>
-      <c r="D57" s="22" t="s">
-        <v>73</v>
-      </c>
-      <c r="E57" s="28"/>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A58" s="35" t="s">
-        <v>131</v>
-      </c>
-      <c r="B58" s="28" t="s">
-        <v>115</v>
-      </c>
-      <c r="D58" s="35" t="s">
-        <v>131</v>
-      </c>
-      <c r="E58" s="28" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A59" s="35" t="s">
-        <v>132</v>
-      </c>
-      <c r="B59" s="28" t="s">
-        <v>116</v>
-      </c>
-      <c r="D59" s="35" t="s">
-        <v>132</v>
-      </c>
-      <c r="E59" s="28" t="s">
+      <c r="D57" s="25"/>
+      <c r="E57" s="29"/>
+    </row>
+    <row r="58" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="59" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A59" s="31" t="s">
+        <v>65</v>
+      </c>
+      <c r="B59" s="26" t="s">
+        <v>100</v>
+      </c>
+      <c r="D59" s="31" t="s">
+        <v>65</v>
+      </c>
+      <c r="E59" s="26" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A60" s="32" t="s">
+        <v>66</v>
+      </c>
+      <c r="B60" s="27"/>
+      <c r="D60" s="32" t="s">
+        <v>66</v>
+      </c>
+      <c r="E60" s="27"/>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A61" s="33" t="s">
+        <v>67</v>
+      </c>
+      <c r="B61" s="28" t="s">
+        <v>100</v>
+      </c>
+      <c r="D61" s="33" t="s">
+        <v>67</v>
+      </c>
+      <c r="E61" s="28" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A60" s="35"/>
-      <c r="B60" s="28"/>
-      <c r="D60" s="24"/>
-      <c r="E60" s="28"/>
-    </row>
-    <row r="61" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A61" s="35"/>
-      <c r="B61" s="28"/>
-      <c r="D61" s="25"/>
-      <c r="E61" s="29"/>
-    </row>
-    <row r="62" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="63" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A63" s="31" t="s">
-        <v>65</v>
-      </c>
-      <c r="B63" s="26" t="s">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A62" s="33" t="s">
+        <v>68</v>
+      </c>
+      <c r="B62" s="28" t="s">
+        <v>87</v>
+      </c>
+      <c r="D62" s="33" t="s">
+        <v>68</v>
+      </c>
+      <c r="E62" s="28" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A63" s="33" t="s">
+        <v>118</v>
+      </c>
+      <c r="B63" s="28" t="s">
+        <v>127</v>
+      </c>
+      <c r="D63" s="33" t="s">
+        <v>118</v>
+      </c>
+      <c r="E63" s="28" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A64" s="33" t="s">
         <v>119</v>
       </c>
-      <c r="D63" s="31" t="s">
-        <v>65</v>
-      </c>
-      <c r="E63" s="26" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A64" s="32" t="s">
-        <v>66</v>
-      </c>
-      <c r="B64" s="27"/>
-      <c r="D64" s="32" t="s">
-        <v>66</v>
-      </c>
-      <c r="E64" s="27"/>
-    </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A65" s="33" t="s">
-        <v>67</v>
+      <c r="B64" s="28" t="s">
+        <v>128</v>
+      </c>
+      <c r="D64" s="33" t="s">
+        <v>119</v>
+      </c>
+      <c r="E64" s="28" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A65" s="34" t="s">
+        <v>69</v>
       </c>
       <c r="B65" s="28" t="s">
-        <v>119</v>
-      </c>
-      <c r="D65" s="33" t="s">
-        <v>67</v>
+        <v>82</v>
+      </c>
+      <c r="D65" s="34" t="s">
+        <v>69</v>
       </c>
       <c r="E65" s="28" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A66" s="33" t="s">
-        <v>68</v>
+        <v>89</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A66" s="34" t="s">
+        <v>70</v>
       </c>
       <c r="B66" s="28" t="s">
-        <v>106</v>
-      </c>
-      <c r="D66" s="33" t="s">
-        <v>68</v>
+        <v>75</v>
+      </c>
+      <c r="D66" s="34" t="s">
+        <v>137</v>
       </c>
       <c r="E66" s="28" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="67" spans="1:5" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A67" s="33" t="s">
-        <v>142</v>
+        <v>138</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A67" s="34" t="s">
+        <v>71</v>
       </c>
       <c r="B67" s="28" t="s">
-        <v>154</v>
-      </c>
-      <c r="D67" s="33" t="s">
-        <v>142</v>
+        <v>101</v>
+      </c>
+      <c r="D67" s="34" t="s">
+        <v>71</v>
       </c>
       <c r="E67" s="28" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A68" s="33" t="s">
-        <v>144</v>
-      </c>
-      <c r="B68" s="28" t="s">
-        <v>155</v>
-      </c>
-      <c r="D68" s="33" t="s">
-        <v>144</v>
-      </c>
-      <c r="E68" s="28" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A69" s="34" t="s">
-        <v>69</v>
+        <v>139</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A68" s="34" t="s">
+        <v>72</v>
+      </c>
+      <c r="B68" s="28"/>
+      <c r="D68" s="34" t="s">
+        <v>72</v>
+      </c>
+      <c r="E68" s="28"/>
+    </row>
+    <row r="69" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A69" s="35" t="s">
+        <v>74</v>
       </c>
       <c r="B69" s="28" t="s">
-        <v>88</v>
-      </c>
-      <c r="D69" s="34" t="s">
-        <v>69</v>
-      </c>
-      <c r="E69" s="28" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A70" s="34" t="s">
-        <v>70</v>
+        <v>92</v>
+      </c>
+      <c r="D69" s="35"/>
+      <c r="E69" s="28"/>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A70" s="35" t="s">
+        <v>76</v>
       </c>
       <c r="B70" s="28" t="s">
-        <v>75</v>
-      </c>
-      <c r="D70" s="34" t="s">
-        <v>168</v>
-      </c>
-      <c r="E70" s="28" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A71" s="34" t="s">
-        <v>71</v>
+        <v>93</v>
+      </c>
+      <c r="D70" s="35"/>
+      <c r="E70" s="28"/>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A71" s="35" t="s">
+        <v>77</v>
       </c>
       <c r="B71" s="28" t="s">
-        <v>120</v>
-      </c>
-      <c r="D71" s="34" t="s">
-        <v>71</v>
-      </c>
-      <c r="E71" s="28" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A72" s="34" t="s">
-        <v>72</v>
-      </c>
-      <c r="B72" s="28"/>
-      <c r="D72" s="34" t="s">
-        <v>72</v>
-      </c>
+        <v>94</v>
+      </c>
+      <c r="D71" s="35"/>
+      <c r="E71" s="28"/>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A72" s="35" t="s">
+        <v>78</v>
+      </c>
+      <c r="B72" s="28" t="s">
+        <v>95</v>
+      </c>
+      <c r="D72" s="35"/>
       <c r="E72" s="28"/>
     </row>
-    <row r="73" spans="1:5" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" s="35" t="s">
-        <v>74</v>
+        <v>102</v>
       </c>
       <c r="B73" s="28" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="D73" s="35"/>
       <c r="E73" s="28"/>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" s="35" t="s">
-        <v>76</v>
+        <v>104</v>
       </c>
       <c r="B74" s="28" t="s">
-        <v>112</v>
+        <v>105</v>
       </c>
       <c r="D74" s="35"/>
       <c r="E74" s="28"/>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A75" s="35" t="s">
-        <v>77</v>
-      </c>
-      <c r="B75" s="28" t="s">
-        <v>113</v>
-      </c>
-      <c r="D75" s="35"/>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A75" s="34" t="s">
+        <v>73</v>
+      </c>
+      <c r="B75" s="28"/>
+      <c r="D75" s="34"/>
       <c r="E75" s="28"/>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" s="35" t="s">
-        <v>78</v>
+        <v>108</v>
       </c>
       <c r="B76" s="28" t="s">
-        <v>114</v>
+        <v>96</v>
       </c>
       <c r="D76" s="35"/>
       <c r="E76" s="28"/>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" s="35" t="s">
-        <v>121</v>
+        <v>109</v>
       </c>
       <c r="B77" s="28" t="s">
-        <v>122</v>
+        <v>97</v>
       </c>
       <c r="D77" s="35"/>
       <c r="E77" s="28"/>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" s="35" t="s">
-        <v>123</v>
+        <v>79</v>
       </c>
       <c r="B78" s="28" t="s">
-        <v>124</v>
+        <v>98</v>
       </c>
       <c r="D78" s="35"/>
       <c r="E78" s="28"/>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A79" s="34" t="s">
-        <v>73</v>
-      </c>
-      <c r="B79" s="28"/>
-      <c r="D79" s="34"/>
-      <c r="E79" s="28"/>
-    </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A79" s="35" t="s">
+        <v>113</v>
+      </c>
+      <c r="B79" s="28" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" s="35" t="s">
+        <v>114</v>
+      </c>
+      <c r="B80" s="28" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A81" s="35" t="s">
+        <v>115</v>
+      </c>
+      <c r="B81" s="28" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="83" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A83" s="31" t="s">
+        <v>65</v>
+      </c>
+      <c r="B83" s="26" t="s">
+        <v>130</v>
+      </c>
+      <c r="D83" s="31" t="s">
+        <v>65</v>
+      </c>
+      <c r="E83" s="26" t="s">
         <v>131</v>
       </c>
-      <c r="B80" s="28" t="s">
-        <v>115</v>
-      </c>
-      <c r="D80" s="35"/>
-      <c r="E80" s="28"/>
-    </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A81" s="35" t="s">
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A84" s="32" t="s">
+        <v>66</v>
+      </c>
+      <c r="B84" s="27"/>
+      <c r="D84" s="32" t="s">
+        <v>66</v>
+      </c>
+      <c r="E84" s="27"/>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A85" s="33" t="s">
+        <v>67</v>
+      </c>
+      <c r="B85" s="28"/>
+      <c r="D85" s="33" t="s">
+        <v>67</v>
+      </c>
+      <c r="E85" s="28"/>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A86" s="33" t="s">
+        <v>68</v>
+      </c>
+      <c r="B86" s="28"/>
+      <c r="D86" s="33" t="s">
+        <v>68</v>
+      </c>
+      <c r="E86" s="28"/>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A87" s="33" t="s">
+        <v>118</v>
+      </c>
+      <c r="B87" s="28"/>
+      <c r="D87" s="33" t="s">
+        <v>118</v>
+      </c>
+      <c r="E87" s="28"/>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A88" s="33" t="s">
+        <v>119</v>
+      </c>
+      <c r="B88" s="28"/>
+      <c r="D88" s="33" t="s">
+        <v>119</v>
+      </c>
+      <c r="E88" s="28"/>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A89" s="34" t="s">
+        <v>69</v>
+      </c>
+      <c r="B89" s="28"/>
+      <c r="D89" s="34" t="s">
+        <v>69</v>
+      </c>
+      <c r="E89" s="28"/>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A90" s="34" t="s">
+        <v>70</v>
+      </c>
+      <c r="B90" s="28"/>
+      <c r="D90" s="34" t="s">
+        <v>70</v>
+      </c>
+      <c r="E90" s="28"/>
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A91" s="34" t="s">
+        <v>71</v>
+      </c>
+      <c r="B91" s="28"/>
+      <c r="D91" s="34" t="s">
+        <v>71</v>
+      </c>
+      <c r="E91" s="28"/>
+    </row>
+    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A92" s="34" t="s">
+        <v>72</v>
+      </c>
+      <c r="B92" s="28"/>
+      <c r="D92" s="34" t="s">
+        <v>72</v>
+      </c>
+      <c r="E92" s="28"/>
+    </row>
+    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A93" s="35"/>
+      <c r="B93" s="28"/>
+      <c r="D93" s="35"/>
+      <c r="E93" s="28"/>
+    </row>
+    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A94" s="35"/>
+      <c r="B94" s="28"/>
+      <c r="D94" s="35"/>
+      <c r="E94" s="28"/>
+    </row>
+    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A95" s="35"/>
+      <c r="B95" s="28"/>
+      <c r="D95" s="35"/>
+      <c r="E95" s="28"/>
+    </row>
+    <row r="96" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="97" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A97" s="31" t="s">
+        <v>65</v>
+      </c>
+      <c r="B97" s="26" t="s">
         <v>132</v>
       </c>
-      <c r="B81" s="28" t="s">
-        <v>116</v>
-      </c>
-      <c r="D81" s="35"/>
-      <c r="E81" s="28"/>
-    </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A82" s="35" t="s">
-        <v>82</v>
-      </c>
-      <c r="B82" s="28" t="s">
-        <v>117</v>
-      </c>
-      <c r="D82" s="35"/>
-      <c r="E82" s="28"/>
-    </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A83" s="35" t="s">
-        <v>136</v>
-      </c>
-      <c r="B83" s="28" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A84" s="35" t="s">
-        <v>137</v>
-      </c>
-      <c r="B84" s="28" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A85" s="35" t="s">
-        <v>138</v>
-      </c>
-      <c r="B85" s="28" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="86" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="87" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A87" s="31" t="s">
-        <v>65</v>
-      </c>
-      <c r="B87" s="26" t="s">
-        <v>157</v>
-      </c>
-      <c r="D87" s="31" t="s">
-        <v>65</v>
-      </c>
-      <c r="E87" s="26" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A88" s="32" t="s">
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A98" s="32" t="s">
         <v>66</v>
       </c>
-      <c r="B88" s="27"/>
-      <c r="D88" s="32" t="s">
-        <v>66</v>
-      </c>
-      <c r="E88" s="27"/>
-    </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A89" s="33" t="s">
+      <c r="B98" s="27"/>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A99" s="33" t="s">
         <v>67</v>
       </c>
-      <c r="B89" s="28"/>
-      <c r="D89" s="33" t="s">
-        <v>67</v>
-      </c>
-      <c r="E89" s="28"/>
-    </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A90" s="33" t="s">
+      <c r="B99" s="28"/>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A100" s="33" t="s">
         <v>68</v>
       </c>
-      <c r="B90" s="28"/>
-      <c r="D90" s="33" t="s">
-        <v>68</v>
-      </c>
-      <c r="E90" s="28"/>
-    </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A91" s="33" t="s">
-        <v>142</v>
-      </c>
-      <c r="B91" s="28"/>
-      <c r="D91" s="33" t="s">
-        <v>142</v>
-      </c>
-      <c r="E91" s="28"/>
-    </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A92" s="33" t="s">
-        <v>144</v>
-      </c>
-      <c r="B92" s="28"/>
-      <c r="D92" s="33" t="s">
-        <v>144</v>
-      </c>
-      <c r="E92" s="28"/>
-    </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A93" s="34" t="s">
+      <c r="B100" s="28"/>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A101" s="33" t="s">
+        <v>118</v>
+      </c>
+      <c r="B101" s="28"/>
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A102" s="33" t="s">
+        <v>119</v>
+      </c>
+      <c r="B102" s="28"/>
+    </row>
+    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A103" s="34" t="s">
         <v>69</v>
       </c>
-      <c r="B93" s="28"/>
-      <c r="D93" s="34" t="s">
-        <v>69</v>
-      </c>
-      <c r="E93" s="28"/>
-    </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A94" s="34" t="s">
+      <c r="B103" s="28"/>
+    </row>
+    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A104" s="34" t="s">
         <v>70</v>
       </c>
-      <c r="B94" s="28"/>
-      <c r="D94" s="34" t="s">
-        <v>70</v>
-      </c>
-      <c r="E94" s="28"/>
-    </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A95" s="34" t="s">
+      <c r="B104" s="28"/>
+    </row>
+    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A105" s="34" t="s">
         <v>71</v>
       </c>
-      <c r="B95" s="28"/>
-      <c r="D95" s="34" t="s">
-        <v>71</v>
-      </c>
-      <c r="E95" s="28"/>
-    </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A96" s="34" t="s">
+      <c r="B105" s="28"/>
+    </row>
+    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A106" s="34" t="s">
         <v>72</v>
       </c>
-      <c r="B96" s="28"/>
-      <c r="D96" s="34" t="s">
-        <v>72</v>
-      </c>
-      <c r="E96" s="28"/>
-    </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A97" s="35"/>
-      <c r="B97" s="28"/>
-      <c r="D97" s="35"/>
-      <c r="E97" s="28"/>
-    </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A98" s="35"/>
-      <c r="B98" s="28"/>
-      <c r="D98" s="35"/>
-      <c r="E98" s="28"/>
-    </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A99" s="35"/>
-      <c r="B99" s="28"/>
-      <c r="D99" s="35"/>
-      <c r="E99" s="28"/>
-    </row>
-    <row r="100" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="101" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A101" s="31" t="s">
-        <v>65</v>
-      </c>
-      <c r="B101" s="26" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A102" s="32" t="s">
-        <v>66</v>
-      </c>
-      <c r="B102" s="27"/>
-    </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A103" s="33" t="s">
-        <v>67</v>
-      </c>
-      <c r="B103" s="28"/>
-    </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A104" s="33" t="s">
-        <v>68</v>
-      </c>
-      <c r="B104" s="28"/>
-    </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A105" s="33" t="s">
-        <v>142</v>
-      </c>
-      <c r="B105" s="28"/>
-    </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A106" s="33" t="s">
-        <v>144</v>
-      </c>
       <c r="B106" s="28"/>
     </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A107" s="34" t="s">
-        <v>69</v>
-      </c>
+    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A107" s="35"/>
       <c r="B107" s="28"/>
     </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A108" s="34" t="s">
-        <v>70</v>
-      </c>
+    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A108" s="35"/>
       <c r="B108" s="28"/>
     </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A109" s="34" t="s">
-        <v>71</v>
-      </c>
+    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A109" s="35"/>
       <c r="B109" s="28"/>
     </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A110" s="34" t="s">
-        <v>72</v>
-      </c>
-      <c r="B110" s="28"/>
-    </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A111" s="35"/>
-      <c r="B111" s="28"/>
-    </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A112" s="35"/>
-      <c r="B112" s="28"/>
-    </row>
-    <row r="113" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A113" s="35"/>
-      <c r="B113" s="28"/>
-    </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="G23:G32"/>
-  </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>